<commit_message>
(JMT) Cleaned up my blocks by removing .project       files.
</commit_message>
<xml_diff>
--- a/blocks/bl_1s4/bl_1s4.xlsx
+++ b/blocks/bl_1s4/bl_1s4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Foretellix\Files\workspace\AV_ValidationVerification\blocks\bl_1s4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BABD6C-0776-4893-B029-DF64730D7BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07790A86-BD94-4B13-8310-CED73C4054FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4935" yWindow="5115" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bl_1s6" sheetId="1" r:id="rId1"/>
@@ -923,7 +923,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>